<commit_message>
Changing Objective Funtion on Retrocalc_Austin routine. Plotting simulation results correctly.
</commit_message>
<xml_diff>
--- a/dados/input.xlsx
+++ b/dados/input.xlsx
@@ -139,10 +139,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -241,7 +241,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Calculating experimental granulometric distributions correctly.
</commit_message>
<xml_diff>
--- a/dados/input.xlsx
+++ b/dados/input.xlsx
@@ -98,17 +98,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -139,17 +135,17 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,34 +169,36 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="0" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.425</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.212</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="G3" s="1" t="n">
         <v>0.106</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>0.053</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.038</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -210,7 +208,6 @@
         <v>0</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -237,209 +234,238 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2"/>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="n">
         <v>66.4798777381559</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="C6" s="3" t="n">
         <v>28.7824758023434</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="D6" s="3" t="n">
         <v>1.78298522669384</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.76413652572593</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="F6" s="3" t="n">
         <v>0.713194090677535</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="G6" s="3" t="n">
         <v>0.254712175241977</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="H6" s="3" t="n">
         <v>0.356597045338767</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="I6" s="3" t="n">
         <v>0.203769740193581</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="J6" s="3" t="n">
         <v>0.662251655629139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="3" t="n">
         <v>51.2809921234709</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="C7" s="3" t="n">
         <v>36.083938076775</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>5.00849613683944</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="E7" s="3" t="n">
         <v>3.07339535669693</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="F7" s="3" t="n">
         <v>1.47978294952074</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>0.68297674593265</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="H7" s="3" t="n">
         <v>0.853720932415813</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="I7" s="3" t="n">
         <v>0.227658915310884</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="J7" s="3" t="n">
         <v>1.30903876303758</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="n">
         <v>34.568222757558</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="C8" s="3" t="n">
         <v>36.4932612800313</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="D8" s="3" t="n">
         <v>9.73153634134167</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="E8" s="3" t="n">
         <v>7.68279184842763</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="F8" s="3" t="n">
         <v>4.73772163986371</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="G8" s="3" t="n">
         <v>2.04874449291403</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="H8" s="3" t="n">
         <v>2.56093061614254</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="I8" s="3" t="n">
         <v>0.256093061614254</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="J8" s="3" t="n">
         <v>1.92069796210691</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="n">
         <v>25.9384649336671</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="C9" s="3" t="n">
         <v>35.3288780585835</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="D9" s="3" t="n">
         <v>11.9719121660316</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="E9" s="3" t="n">
         <v>9.97659347169302</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="F9" s="3" t="n">
         <v>5.16435426769992</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <v>2.58217713384996</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="H9" s="3" t="n">
         <v>3.16903557336131</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="I9" s="3" t="n">
         <v>0.938973503218167</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="J9" s="3" t="n">
         <v>4.92961089189538</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
+      <c r="A10" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="n">
         <v>16.3607968584373</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="C10" s="3" t="n">
         <v>27.9554945282941</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="D10" s="3" t="n">
         <v>13.977747264147</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="E10" s="3" t="n">
         <v>14.2050277074665</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="F10" s="3" t="n">
         <v>7.95481551618124</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="G10" s="3" t="n">
         <v>4.09104797975035</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="H10" s="3" t="n">
         <v>6.13657196962553</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="I10" s="3" t="n">
         <v>2.04552398987517</v>
       </c>
-      <c r="I10" s="4" t="n">
+      <c r="J10" s="3" t="n">
         <v>7.27297418622284</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="n">
         <v>10.0433948459933</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="C11" s="3" t="n">
         <v>21.1383803470427</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="D11" s="3" t="n">
         <v>13.839477716001</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="E11" s="3" t="n">
         <v>16.1144603542478</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="F11" s="3" t="n">
         <v>10.0478399855898</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="G11" s="3" t="n">
         <v>5.59266565235658</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="H11" s="3" t="n">
         <v>8.53118489342529</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="I11" s="3" t="n">
         <v>2.84372829780843</v>
       </c>
-      <c r="I11" s="4" t="n">
+      <c r="J11" s="3" t="n">
         <v>11.8488679075351</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Making some cleaning. Starting cinetic fit optimization.
</commit_message>
<xml_diff>
--- a/dados/input.xlsx
+++ b/dados/input.xlsx
@@ -21,17 +21,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -98,7 +98,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -112,6 +112,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -124,6 +136,15 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -132,13 +153,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -243,7 +264,7 @@
       <c r="A5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -467,12 +488,180 @@
       </c>
       <c r="J11" s="3" t="n">
         <v>11.8488679075351</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>1180</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>840</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>600</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>425</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>300</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>212</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>106</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="J15" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="L15" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>98.7369389776355</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>96.3662705971974</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>91.8192509166852</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>80.8014724600592</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>57.4097934667296</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>34.9327641511757</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>20.8043457242561</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>10.8988843202588</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>6.38401782570595</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <v>4.00982078977732</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>3.8930570011251</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>98.3333333333333</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>98.3333333333333</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>98.3333333333333</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>95</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>73.3333333333333</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>36.6666666666667</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>23.3333333333333</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>16.6666666666667</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <v>11.6666666666667</v>
+      </c>
+      <c r="L17" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>97.9166666666667</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>97.9166666666667</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>97.9166666666667</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>95.8333333333333</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>79.1666666666667</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>56.25</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <v>41.6666666666667</v>
+      </c>
+      <c r="I18" s="6" t="n">
+        <v>27.0833333333333</v>
+      </c>
+      <c r="J18" s="6" t="n">
+        <v>18.75</v>
+      </c>
+      <c r="K18" s="6" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L18" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
first optimization -> opt_cf_1
</commit_message>
<xml_diff>
--- a/dados/input.xlsx
+++ b/dados/input.xlsx
@@ -32,6 +32,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,15 +137,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -159,7 +151,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">

</xml_diff>